<commit_message>
feat: process excel and get the insert sql
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opensource\region-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5616C5C-E9B1-4B5F-85E5-A3C6ECA97061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A148B7F-EFAA-4A93-A735-A394460CD313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7305" yWindow="3525" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="劝导站统计" sheetId="2" r:id="rId1"/>
+    <sheet name="村居统计" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>县</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +57,30 @@
   </si>
   <si>
     <t>山王</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>程店村检查站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烟店村检查站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山王检查站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>县区名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乡镇名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村居名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -63,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,16 +405,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA1724-3E29-4A6F-B59F-025E8972747E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -411,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -422,7 +508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
feat: add regionTree api and relation functions
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opensource\region-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A148B7F-EFAA-4A93-A735-A394460CD313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA792B7-06E6-4504-897D-0CF551BA7B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="3525" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3405" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="劝导站统计" sheetId="2" r:id="rId1"/>
@@ -26,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
-  <si>
-    <t>县</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>乡镇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>村</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>肥西县</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -408,54 +396,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA1724-3E29-4A6F-B59F-025E8972747E}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -469,54 +457,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: api with pCode and type params issue fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opensource\region-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA792B7-06E6-4504-897D-0CF551BA7B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5801DC-8F27-4A13-8C6F-738CF42CAB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="劝导站统计" sheetId="2" r:id="rId1"/>
@@ -26,39 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
-  <si>
-    <t>肥西县</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>丰乐镇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>程店村</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟店村</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>山王</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>程店村检查站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟店村检查站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>山王检查站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
   <si>
     <t>县区名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +37,130 @@
   </si>
   <si>
     <t>村居名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村子2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村子3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镇1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>县1</t>
+  </si>
+  <si>
+    <t>县1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镇2</t>
+  </si>
+  <si>
+    <t>镇2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村子4</t>
+  </si>
+  <si>
+    <t>村子5</t>
+  </si>
+  <si>
+    <t>村子6</t>
+  </si>
+  <si>
+    <t>村子7</t>
+  </si>
+  <si>
+    <t>村子8</t>
+  </si>
+  <si>
+    <t>村子9</t>
+  </si>
+  <si>
+    <t>村子10</t>
+  </si>
+  <si>
+    <t>村子11</t>
+  </si>
+  <si>
+    <t>村子12</t>
+  </si>
+  <si>
+    <t>村子13</t>
+  </si>
+  <si>
+    <t>村子1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村子14</t>
+  </si>
+  <si>
+    <t>村子15</t>
+  </si>
+  <si>
+    <t>县2</t>
+  </si>
+  <si>
+    <t>镇3</t>
+  </si>
+  <si>
+    <t>镇3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查点1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查点2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查点3</t>
+  </si>
+  <si>
+    <t>检查点4</t>
+  </si>
+  <si>
+    <t>检查点5</t>
+  </si>
+  <si>
+    <t>检查点6</t>
+  </si>
+  <si>
+    <t>检查点7</t>
+  </si>
+  <si>
+    <t>检查点8</t>
+  </si>
+  <si>
+    <t>检查点9</t>
+  </si>
+  <si>
+    <t>检查点10</t>
+  </si>
+  <si>
+    <t>检查点11</t>
+  </si>
+  <si>
+    <t>检查点12</t>
+  </si>
+  <si>
+    <t>检查点13</t>
+  </si>
+  <si>
+    <t>检查点14</t>
+  </si>
+  <si>
+    <t>检查点15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -394,7 +486,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA1724-3E29-4A6F-B59F-025E8972747E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1"/>
@@ -404,107 +689,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add counselor insert sql process
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opensource\region-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5801DC-8F27-4A13-8C6F-738CF42CAB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18A8763-CC1D-4A26-B954-A98EA9584525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
   <si>
     <t>县区名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -162,6 +162,123 @@
   <si>
     <t>检查点15</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入职时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三3</t>
+  </si>
+  <si>
+    <t>张三4</t>
+  </si>
+  <si>
+    <t>张三5</t>
+  </si>
+  <si>
+    <t>张三6</t>
+  </si>
+  <si>
+    <t>张三7</t>
+  </si>
+  <si>
+    <t>张三8</t>
+  </si>
+  <si>
+    <t>张三9</t>
+  </si>
+  <si>
+    <t>张三10</t>
+  </si>
+  <si>
+    <t>张三11</t>
+  </si>
+  <si>
+    <t>张三12</t>
+  </si>
+  <si>
+    <t>张三13</t>
+  </si>
+  <si>
+    <t>张三14</t>
+  </si>
+  <si>
+    <t>张三15</t>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务2</t>
+  </si>
+  <si>
+    <t>职务3</t>
+  </si>
+  <si>
+    <t>职务4</t>
+  </si>
+  <si>
+    <t>职务5</t>
+  </si>
+  <si>
+    <t>职务6</t>
+  </si>
+  <si>
+    <t>职务7</t>
+  </si>
+  <si>
+    <t>职务8</t>
+  </si>
+  <si>
+    <t>职务9</t>
+  </si>
+  <si>
+    <t>职务10</t>
+  </si>
+  <si>
+    <t>职务11</t>
+  </si>
+  <si>
+    <t>职务12</t>
+  </si>
+  <si>
+    <t>职务13</t>
+  </si>
+  <si>
+    <t>职务14</t>
+  </si>
+  <si>
+    <t>职务15</t>
   </si>
 </sst>
 </file>
@@ -204,8 +321,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -486,15 +604,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA1724-3E29-4A6F-B59F-025E8972747E}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +625,23 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -515,8 +651,23 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -526,8 +677,23 @@
       <c r="C3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -537,8 +703,23 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>125</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -548,8 +729,23 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>126</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -559,8 +755,23 @@
       <c r="C6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -570,8 +781,23 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -581,8 +807,23 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>129</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="1">
+        <v>44517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -592,8 +833,23 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>130</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="1">
+        <v>44518</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -603,8 +859,23 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>131</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="1">
+        <v>44519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -614,8 +885,23 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="1">
+        <v>44520</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -625,8 +911,23 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1">
+        <v>44521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -636,8 +937,23 @@
       <c r="C13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="1">
+        <v>44522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -647,8 +963,23 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>135</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="1">
+        <v>44523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -658,8 +989,23 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="1">
+        <v>44524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -668,6 +1014,21 @@
       </c>
       <c r="C16" t="s">
         <v>40</v>
+      </c>
+      <c r="D16">
+        <v>137</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="1">
+        <v>44525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(bug): when two village have same names in different town, only add one.
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Opensource\region-demo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18A8763-CC1D-4A26-B954-A98EA9584525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68A49B8-E176-46E9-8709-A32A2F88C83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35835" yWindow="1590" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="劝导站统计" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>县区名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,158 +127,156 @@
     <t>检查点3</t>
   </si>
   <si>
+    <t>检查点5</t>
+  </si>
+  <si>
+    <t>检查点6</t>
+  </si>
+  <si>
+    <t>检查点7</t>
+  </si>
+  <si>
+    <t>检查点8</t>
+  </si>
+  <si>
+    <t>检查点9</t>
+  </si>
+  <si>
+    <t>检查点10</t>
+  </si>
+  <si>
+    <t>检查点11</t>
+  </si>
+  <si>
+    <t>检查点13</t>
+  </si>
+  <si>
+    <t>检查点14</t>
+  </si>
+  <si>
+    <t>检查点15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入职时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三3</t>
+  </si>
+  <si>
+    <t>张三4</t>
+  </si>
+  <si>
+    <t>张三5</t>
+  </si>
+  <si>
+    <t>张三6</t>
+  </si>
+  <si>
+    <t>张三7</t>
+  </si>
+  <si>
+    <t>张三8</t>
+  </si>
+  <si>
+    <t>张三9</t>
+  </si>
+  <si>
+    <t>张三10</t>
+  </si>
+  <si>
+    <t>张三11</t>
+  </si>
+  <si>
+    <t>张三12</t>
+  </si>
+  <si>
+    <t>张三13</t>
+  </si>
+  <si>
+    <t>张三14</t>
+  </si>
+  <si>
+    <t>张三15</t>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职务2</t>
+  </si>
+  <si>
+    <t>职务3</t>
+  </si>
+  <si>
+    <t>职务4</t>
+  </si>
+  <si>
+    <t>职务5</t>
+  </si>
+  <si>
+    <t>职务6</t>
+  </si>
+  <si>
+    <t>职务7</t>
+  </si>
+  <si>
+    <t>职务8</t>
+  </si>
+  <si>
+    <t>职务9</t>
+  </si>
+  <si>
+    <t>职务10</t>
+  </si>
+  <si>
+    <t>职务11</t>
+  </si>
+  <si>
+    <t>职务12</t>
+  </si>
+  <si>
+    <t>职务13</t>
+  </si>
+  <si>
+    <t>职务14</t>
+  </si>
+  <si>
+    <t>职务15</t>
+  </si>
+  <si>
     <t>检查点4</t>
-  </si>
-  <si>
-    <t>检查点5</t>
-  </si>
-  <si>
-    <t>检查点6</t>
-  </si>
-  <si>
-    <t>检查点7</t>
-  </si>
-  <si>
-    <t>检查点8</t>
-  </si>
-  <si>
-    <t>检查点9</t>
-  </si>
-  <si>
-    <t>检查点10</t>
-  </si>
-  <si>
-    <t>检查点11</t>
-  </si>
-  <si>
-    <t>检查点12</t>
-  </si>
-  <si>
-    <t>检查点13</t>
-  </si>
-  <si>
-    <t>检查点14</t>
-  </si>
-  <si>
-    <t>检查点15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>入职时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张三1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张三2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张三3</t>
-  </si>
-  <si>
-    <t>张三4</t>
-  </si>
-  <si>
-    <t>张三5</t>
-  </si>
-  <si>
-    <t>张三6</t>
-  </si>
-  <si>
-    <t>张三7</t>
-  </si>
-  <si>
-    <t>张三8</t>
-  </si>
-  <si>
-    <t>张三9</t>
-  </si>
-  <si>
-    <t>张三10</t>
-  </si>
-  <si>
-    <t>张三11</t>
-  </si>
-  <si>
-    <t>张三12</t>
-  </si>
-  <si>
-    <t>张三13</t>
-  </si>
-  <si>
-    <t>张三14</t>
-  </si>
-  <si>
-    <t>张三15</t>
-  </si>
-  <si>
-    <t>男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职务1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职务2</t>
-  </si>
-  <si>
-    <t>职务3</t>
-  </si>
-  <si>
-    <t>职务4</t>
-  </si>
-  <si>
-    <t>职务5</t>
-  </si>
-  <si>
-    <t>职务6</t>
-  </si>
-  <si>
-    <t>职务7</t>
-  </si>
-  <si>
-    <t>职务8</t>
-  </si>
-  <si>
-    <t>职务9</t>
-  </si>
-  <si>
-    <t>职务10</t>
-  </si>
-  <si>
-    <t>职务11</t>
-  </si>
-  <si>
-    <t>职务12</t>
-  </si>
-  <si>
-    <t>职务13</t>
-  </si>
-  <si>
-    <t>职务14</t>
-  </si>
-  <si>
-    <t>职务15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -607,7 +605,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -626,19 +624,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -655,13 +653,13 @@
         <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>44511</v>
@@ -681,13 +679,13 @@
         <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
       </c>
       <c r="H3" s="1">
         <v>44512</v>
@@ -707,13 +705,13 @@
         <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" s="1">
         <v>44513</v>
@@ -727,19 +725,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H5" s="1">
         <v>44514</v>
@@ -753,19 +751,19 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" s="1">
         <v>44515</v>
@@ -779,19 +777,19 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H7" s="1">
         <v>44516</v>
@@ -805,19 +803,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H8" s="1">
         <v>44517</v>
@@ -831,19 +829,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H9" s="1">
         <v>44518</v>
@@ -857,19 +855,19 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="1">
         <v>44519</v>
@@ -883,19 +881,19 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H11" s="1">
         <v>44520</v>
@@ -909,19 +907,19 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>133</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H12" s="1">
         <v>44521</v>
@@ -935,19 +933,19 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>134</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1">
         <v>44522</v>
@@ -961,19 +959,19 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>135</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1">
         <v>44523</v>
@@ -987,19 +985,19 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H15" s="1">
         <v>44524</v>
@@ -1013,19 +1011,19 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1">
         <v>44525</v>

</xml_diff>